<commit_message>
updates after the most recent black-box evals.
</commit_message>
<xml_diff>
--- a/Function 2/evals.xlsx
+++ b/Function 2/evals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prithvi\Desktop\Imperial Course\Capstone Project\Function 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prithvi\Desktop\Imperial Course\Capstone-Project\Function 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B93AE1E-542D-4FA2-836A-65F9174AADE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E565BE6-A158-4DD1-B939-F3FD9898A539}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,10 +84,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -376,44 +376,44 @@
   <dimension ref="B2:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="H4" sqref="H4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
         <v>0.71402200000000005</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4">
         <v>0.14477200000000001</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="5">
         <v>0.59747244630609897</v>
       </c>
@@ -422,156 +422,160 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4">
+        <v>0.74275198707938395</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4">
+        <v>0.88397478133732699</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -579,19 +583,20 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -603,10 +608,23 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="F3:G3"/>
@@ -617,20 +635,6 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>